<commit_message>
New structure for CARA patient
</commit_message>
<xml_diff>
--- a/output/all-profiles.xlsx
+++ b/output/all-profiles.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2958" uniqueCount="425">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4493" uniqueCount="430">
   <si>
     <t>Property</t>
   </si>
@@ -63,7 +63,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-07-11T13:23:42+02:00</t>
+    <t>2023-07-11T14:45:02+02:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1357,6 +1357,21 @@
   </si>
   <si>
     <t>Knowing which language a practitioner speaks can help in facilitating communication with patients.</t>
+  </si>
+  <si>
+    <t>cara-patient</t>
+  </si>
+  <si>
+    <t>http://example.org/fhir/fish/StructureDefinition/cara-patient</t>
+  </si>
+  <si>
+    <t>CaraPatient</t>
+  </si>
+  <si>
+    <t>CaraPatient Patient</t>
+  </si>
+  <si>
+    <t>A patient who is affiliated to the CARA community</t>
   </si>
 </sst>
 </file>
@@ -1490,7 +1505,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B61"/>
+  <dimension ref="A1:B81"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -1964,6 +1979,158 @@
         <v>35</v>
       </c>
     </row>
+    <row r="62">
+      <c r="A62" t="s" s="1">
+        <v>0</v>
+      </c>
+      <c r="B62" t="s" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="s" s="2">
+        <v>2</v>
+      </c>
+      <c r="B63" t="s" s="2">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="s" s="2">
+        <v>4</v>
+      </c>
+      <c r="B64" t="s" s="2">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="s" s="2">
+        <v>6</v>
+      </c>
+      <c r="B65" t="s" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="B66" t="s" s="2">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="s" s="2">
+        <v>10</v>
+      </c>
+      <c r="B67" t="s" s="2">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="s" s="2">
+        <v>12</v>
+      </c>
+      <c r="B68" t="s" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="B69" s="2"/>
+    </row>
+    <row r="70">
+      <c r="A70" t="s" s="2">
+        <v>15</v>
+      </c>
+      <c r="B70" t="s" s="2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="s" s="2">
+        <v>17</v>
+      </c>
+      <c r="B71" s="2"/>
+    </row>
+    <row r="72">
+      <c r="A72" t="s" s="2">
+        <v>18</v>
+      </c>
+      <c r="B72" t="s" s="2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="B73" t="s" s="2">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="s" s="2">
+        <v>22</v>
+      </c>
+      <c r="B74" s="2"/>
+    </row>
+    <row r="75">
+      <c r="A75" t="s" s="2">
+        <v>23</v>
+      </c>
+      <c r="B75" s="2"/>
+    </row>
+    <row r="76">
+      <c r="A76" t="s" s="2">
+        <v>24</v>
+      </c>
+      <c r="B76" t="s" s="2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="s" s="2">
+        <v>26</v>
+      </c>
+      <c r="B77" t="s" s="2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="s" s="2">
+        <v>28</v>
+      </c>
+      <c r="B78" t="s" s="2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="s" s="2">
+        <v>30</v>
+      </c>
+      <c r="B79" t="s" s="2">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="s" s="2">
+        <v>32</v>
+      </c>
+      <c r="B80" t="s" s="2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="B81" t="s" s="2">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -1971,7 +2138,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AK86"/>
+  <dimension ref="A1:AK131"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -1980,7 +2147,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="11.9140625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="12.046875" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="42.9609375" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="39.57421875" customWidth="true" bestFit="true" hidden="true"/>
     <col min="4" max="4" width="14.2890625" customWidth="true" bestFit="true" hidden="true"/>
@@ -11066,6 +11233,4759 @@
         <v>68</v>
       </c>
     </row>
+    <row r="87">
+      <c r="A87" t="s" s="2">
+        <v>425</v>
+      </c>
+      <c r="B87" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="C87" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="D87" s="2"/>
+      <c r="E87" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="F87" s="2"/>
+      <c r="G87" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="H87" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I87" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="J87" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="K87" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="L87" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="M87" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="N87" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="O87" s="2"/>
+      <c r="P87" s="2"/>
+      <c r="Q87" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="R87" s="2"/>
+      <c r="S87" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="T87" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="U87" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="V87" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="W87" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="X87" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Y87" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Z87" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AA87" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AB87" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AC87" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AD87" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AE87" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AF87" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AG87" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AH87" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI87" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ87" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AK87" t="s" s="2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="s" s="2">
+        <v>425</v>
+      </c>
+      <c r="B88" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="C88" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="D88" s="2"/>
+      <c r="E88" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="F88" s="2"/>
+      <c r="G88" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="H88" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="I88" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="J88" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="K88" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="L88" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="M88" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="N88" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="O88" t="s" s="2">
+        <v>85</v>
+      </c>
+      <c r="P88" s="2"/>
+      <c r="Q88" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="R88" s="2"/>
+      <c r="S88" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="T88" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="U88" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="V88" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="W88" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="X88" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Y88" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Z88" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AA88" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AB88" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AC88" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AD88" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AE88" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AF88" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AG88" t="s" s="2">
+        <v>86</v>
+      </c>
+      <c r="AH88" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI88" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AJ88" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AK88" t="s" s="2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="s" s="2">
+        <v>425</v>
+      </c>
+      <c r="B89" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="C89" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="D89" s="2"/>
+      <c r="E89" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="F89" s="2"/>
+      <c r="G89" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="H89" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="I89" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="J89" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="K89" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="L89" t="s" s="2">
+        <v>88</v>
+      </c>
+      <c r="M89" t="s" s="2">
+        <v>89</v>
+      </c>
+      <c r="N89" t="s" s="2">
+        <v>90</v>
+      </c>
+      <c r="O89" s="2"/>
+      <c r="P89" s="2"/>
+      <c r="Q89" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="R89" s="2"/>
+      <c r="S89" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="T89" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="U89" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="V89" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="W89" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="X89" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Y89" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Z89" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AA89" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AB89" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AC89" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AD89" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AE89" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AF89" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AG89" t="s" s="2">
+        <v>91</v>
+      </c>
+      <c r="AH89" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI89" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AJ89" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AK89" t="s" s="2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="s" s="2">
+        <v>425</v>
+      </c>
+      <c r="B90" t="s" s="2">
+        <v>92</v>
+      </c>
+      <c r="C90" t="s" s="2">
+        <v>92</v>
+      </c>
+      <c r="D90" s="2"/>
+      <c r="E90" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="F90" s="2"/>
+      <c r="G90" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="H90" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="I90" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="J90" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="K90" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="L90" t="s" s="2">
+        <v>58</v>
+      </c>
+      <c r="M90" t="s" s="2">
+        <v>93</v>
+      </c>
+      <c r="N90" t="s" s="2">
+        <v>94</v>
+      </c>
+      <c r="O90" t="s" s="2">
+        <v>95</v>
+      </c>
+      <c r="P90" s="2"/>
+      <c r="Q90" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="R90" s="2"/>
+      <c r="S90" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="T90" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="U90" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="V90" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="W90" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="X90" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Y90" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Z90" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AA90" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AB90" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AC90" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AD90" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AE90" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AF90" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AG90" t="s" s="2">
+        <v>96</v>
+      </c>
+      <c r="AH90" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI90" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AJ90" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AK90" t="s" s="2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="s" s="2">
+        <v>425</v>
+      </c>
+      <c r="B91" t="s" s="2">
+        <v>97</v>
+      </c>
+      <c r="C91" t="s" s="2">
+        <v>97</v>
+      </c>
+      <c r="D91" s="2"/>
+      <c r="E91" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="F91" s="2"/>
+      <c r="G91" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="H91" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="I91" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="J91" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="K91" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="L91" t="s" s="2">
+        <v>98</v>
+      </c>
+      <c r="M91" t="s" s="2">
+        <v>99</v>
+      </c>
+      <c r="N91" t="s" s="2">
+        <v>100</v>
+      </c>
+      <c r="O91" t="s" s="2">
+        <v>101</v>
+      </c>
+      <c r="P91" s="2"/>
+      <c r="Q91" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="R91" s="2"/>
+      <c r="S91" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="T91" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="U91" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="V91" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="W91" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="X91" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Y91" t="s" s="2">
+        <v>102</v>
+      </c>
+      <c r="Z91" t="s" s="2">
+        <v>103</v>
+      </c>
+      <c r="AA91" t="s" s="2">
+        <v>104</v>
+      </c>
+      <c r="AB91" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AC91" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AD91" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AE91" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AF91" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AG91" t="s" s="2">
+        <v>105</v>
+      </c>
+      <c r="AH91" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI91" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AJ91" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AK91" t="s" s="2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="s" s="2">
+        <v>425</v>
+      </c>
+      <c r="B92" t="s" s="2">
+        <v>106</v>
+      </c>
+      <c r="C92" t="s" s="2">
+        <v>106</v>
+      </c>
+      <c r="D92" s="2"/>
+      <c r="E92" t="s" s="2">
+        <v>107</v>
+      </c>
+      <c r="F92" s="2"/>
+      <c r="G92" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="H92" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="I92" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="J92" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="K92" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="L92" t="s" s="2">
+        <v>108</v>
+      </c>
+      <c r="M92" t="s" s="2">
+        <v>109</v>
+      </c>
+      <c r="N92" t="s" s="2">
+        <v>110</v>
+      </c>
+      <c r="O92" t="s" s="2">
+        <v>111</v>
+      </c>
+      <c r="P92" s="2"/>
+      <c r="Q92" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="R92" s="2"/>
+      <c r="S92" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="T92" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="U92" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="V92" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="W92" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="X92" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Y92" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Z92" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AA92" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AB92" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AC92" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AD92" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AE92" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AF92" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AG92" t="s" s="2">
+        <v>112</v>
+      </c>
+      <c r="AH92" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI92" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AJ92" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AK92" t="s" s="2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="s" s="2">
+        <v>425</v>
+      </c>
+      <c r="B93" t="s" s="2">
+        <v>113</v>
+      </c>
+      <c r="C93" t="s" s="2">
+        <v>113</v>
+      </c>
+      <c r="D93" s="2"/>
+      <c r="E93" t="s" s="2">
+        <v>114</v>
+      </c>
+      <c r="F93" s="2"/>
+      <c r="G93" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="H93" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I93" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="J93" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="K93" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="L93" t="s" s="2">
+        <v>115</v>
+      </c>
+      <c r="M93" t="s" s="2">
+        <v>116</v>
+      </c>
+      <c r="N93" t="s" s="2">
+        <v>117</v>
+      </c>
+      <c r="O93" t="s" s="2">
+        <v>118</v>
+      </c>
+      <c r="P93" s="2"/>
+      <c r="Q93" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="R93" s="2"/>
+      <c r="S93" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="T93" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="U93" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="V93" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="W93" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="X93" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Y93" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Z93" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AA93" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AB93" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AC93" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AD93" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AE93" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AF93" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AG93" t="s" s="2">
+        <v>119</v>
+      </c>
+      <c r="AH93" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI93" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ93" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AK93" t="s" s="2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="s" s="2">
+        <v>425</v>
+      </c>
+      <c r="B94" t="s" s="2">
+        <v>120</v>
+      </c>
+      <c r="C94" t="s" s="2">
+        <v>120</v>
+      </c>
+      <c r="D94" s="2"/>
+      <c r="E94" t="s" s="2">
+        <v>126</v>
+      </c>
+      <c r="F94" s="2"/>
+      <c r="G94" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="H94" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I94" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="J94" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="K94" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="L94" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="M94" t="s" s="2">
+        <v>209</v>
+      </c>
+      <c r="N94" t="s" s="2">
+        <v>308</v>
+      </c>
+      <c r="O94" t="s" s="2">
+        <v>129</v>
+      </c>
+      <c r="P94" s="2"/>
+      <c r="Q94" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="R94" s="2"/>
+      <c r="S94" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="T94" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="U94" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="V94" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="W94" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="X94" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Y94" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Z94" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AA94" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AB94" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AC94" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AD94" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AE94" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AF94" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AG94" t="s" s="2">
+        <v>121</v>
+      </c>
+      <c r="AH94" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI94" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ94" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AK94" t="s" s="2">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="s" s="2">
+        <v>425</v>
+      </c>
+      <c r="B95" t="s" s="2">
+        <v>125</v>
+      </c>
+      <c r="C95" t="s" s="2">
+        <v>125</v>
+      </c>
+      <c r="D95" s="2"/>
+      <c r="E95" t="s" s="2">
+        <v>126</v>
+      </c>
+      <c r="F95" s="2"/>
+      <c r="G95" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="H95" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I95" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="J95" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="K95" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="L95" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="M95" t="s" s="2">
+        <v>127</v>
+      </c>
+      <c r="N95" t="s" s="2">
+        <v>128</v>
+      </c>
+      <c r="O95" t="s" s="2">
+        <v>129</v>
+      </c>
+      <c r="P95" t="s" s="2">
+        <v>130</v>
+      </c>
+      <c r="Q95" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="R95" s="2"/>
+      <c r="S95" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="T95" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="U95" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="V95" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="W95" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="X95" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Y95" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Z95" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AA95" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AB95" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AC95" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AD95" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AE95" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AF95" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AG95" t="s" s="2">
+        <v>131</v>
+      </c>
+      <c r="AH95" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI95" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ95" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AK95" t="s" s="2">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="s" s="2">
+        <v>425</v>
+      </c>
+      <c r="B96" t="s" s="2">
+        <v>132</v>
+      </c>
+      <c r="C96" t="s" s="2">
+        <v>132</v>
+      </c>
+      <c r="D96" s="2"/>
+      <c r="E96" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="F96" s="2"/>
+      <c r="G96" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="H96" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I96" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="J96" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="K96" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="L96" t="s" s="2">
+        <v>133</v>
+      </c>
+      <c r="M96" t="s" s="2">
+        <v>134</v>
+      </c>
+      <c r="N96" t="s" s="2">
+        <v>135</v>
+      </c>
+      <c r="O96" s="2"/>
+      <c r="P96" t="s" s="2">
+        <v>136</v>
+      </c>
+      <c r="Q96" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="R96" s="2"/>
+      <c r="S96" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="T96" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="U96" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="V96" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="W96" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="X96" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Y96" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Z96" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AA96" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AB96" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AC96" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AD96" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AE96" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AF96" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AG96" t="s" s="2">
+        <v>132</v>
+      </c>
+      <c r="AH96" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI96" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ96" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AK96" t="s" s="2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="s" s="2">
+        <v>425</v>
+      </c>
+      <c r="B97" t="s" s="2">
+        <v>137</v>
+      </c>
+      <c r="C97" t="s" s="2">
+        <v>137</v>
+      </c>
+      <c r="D97" s="2"/>
+      <c r="E97" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="F97" s="2"/>
+      <c r="G97" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="H97" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="I97" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="J97" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="K97" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="L97" t="s" s="2">
+        <v>138</v>
+      </c>
+      <c r="M97" t="s" s="2">
+        <v>139</v>
+      </c>
+      <c r="N97" t="s" s="2">
+        <v>140</v>
+      </c>
+      <c r="O97" t="s" s="2">
+        <v>141</v>
+      </c>
+      <c r="P97" t="s" s="2">
+        <v>142</v>
+      </c>
+      <c r="Q97" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="R97" t="s" s="2">
+        <v>143</v>
+      </c>
+      <c r="S97" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="T97" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="U97" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="V97" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="W97" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="X97" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Y97" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Z97" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AA97" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AB97" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AC97" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AD97" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AE97" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AF97" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AG97" t="s" s="2">
+        <v>137</v>
+      </c>
+      <c r="AH97" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI97" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AJ97" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AK97" t="s" s="2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="s" s="2">
+        <v>425</v>
+      </c>
+      <c r="B98" t="s" s="2">
+        <v>144</v>
+      </c>
+      <c r="C98" t="s" s="2">
+        <v>144</v>
+      </c>
+      <c r="D98" s="2"/>
+      <c r="E98" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="F98" s="2"/>
+      <c r="G98" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="H98" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I98" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="J98" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="K98" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="L98" t="s" s="2">
+        <v>145</v>
+      </c>
+      <c r="M98" t="s" s="2">
+        <v>146</v>
+      </c>
+      <c r="N98" t="s" s="2">
+        <v>147</v>
+      </c>
+      <c r="O98" t="s" s="2">
+        <v>148</v>
+      </c>
+      <c r="P98" t="s" s="2">
+        <v>149</v>
+      </c>
+      <c r="Q98" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="R98" s="2"/>
+      <c r="S98" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="T98" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="U98" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="V98" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="W98" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="X98" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Y98" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Z98" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AA98" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AB98" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AC98" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AD98" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AE98" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AF98" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AG98" t="s" s="2">
+        <v>144</v>
+      </c>
+      <c r="AH98" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI98" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ98" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AK98" t="s" s="2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="s" s="2">
+        <v>425</v>
+      </c>
+      <c r="B99" t="s" s="2">
+        <v>150</v>
+      </c>
+      <c r="C99" t="s" s="2">
+        <v>150</v>
+      </c>
+      <c r="D99" s="2"/>
+      <c r="E99" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="F99" s="2"/>
+      <c r="G99" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="H99" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I99" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="J99" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="K99" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="L99" t="s" s="2">
+        <v>151</v>
+      </c>
+      <c r="M99" t="s" s="2">
+        <v>152</v>
+      </c>
+      <c r="N99" t="s" s="2">
+        <v>153</v>
+      </c>
+      <c r="O99" t="s" s="2">
+        <v>154</v>
+      </c>
+      <c r="P99" t="s" s="2">
+        <v>155</v>
+      </c>
+      <c r="Q99" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="R99" s="2"/>
+      <c r="S99" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="T99" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="U99" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="V99" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="W99" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="X99" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Y99" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Z99" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AA99" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AB99" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AC99" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AD99" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AE99" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AF99" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AG99" t="s" s="2">
+        <v>150</v>
+      </c>
+      <c r="AH99" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI99" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ99" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AK99" t="s" s="2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="s" s="2">
+        <v>425</v>
+      </c>
+      <c r="B100" t="s" s="2">
+        <v>156</v>
+      </c>
+      <c r="C100" t="s" s="2">
+        <v>156</v>
+      </c>
+      <c r="D100" s="2"/>
+      <c r="E100" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="F100" s="2"/>
+      <c r="G100" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="H100" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="I100" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="J100" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="K100" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="L100" t="s" s="2">
+        <v>98</v>
+      </c>
+      <c r="M100" t="s" s="2">
+        <v>157</v>
+      </c>
+      <c r="N100" t="s" s="2">
+        <v>158</v>
+      </c>
+      <c r="O100" t="s" s="2">
+        <v>159</v>
+      </c>
+      <c r="P100" t="s" s="2">
+        <v>160</v>
+      </c>
+      <c r="Q100" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="R100" s="2"/>
+      <c r="S100" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="T100" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="U100" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="V100" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="W100" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="X100" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Y100" t="s" s="2">
+        <v>161</v>
+      </c>
+      <c r="Z100" t="s" s="2">
+        <v>162</v>
+      </c>
+      <c r="AA100" t="s" s="2">
+        <v>163</v>
+      </c>
+      <c r="AB100" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AC100" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AD100" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AE100" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AF100" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AG100" t="s" s="2">
+        <v>156</v>
+      </c>
+      <c r="AH100" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI100" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AJ100" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AK100" t="s" s="2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="s" s="2">
+        <v>425</v>
+      </c>
+      <c r="B101" t="s" s="2">
+        <v>164</v>
+      </c>
+      <c r="C101" t="s" s="2">
+        <v>164</v>
+      </c>
+      <c r="D101" s="2"/>
+      <c r="E101" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="F101" s="2"/>
+      <c r="G101" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="H101" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="I101" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="J101" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="K101" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="L101" t="s" s="2">
+        <v>165</v>
+      </c>
+      <c r="M101" t="s" s="2">
+        <v>166</v>
+      </c>
+      <c r="N101" t="s" s="2">
+        <v>167</v>
+      </c>
+      <c r="O101" t="s" s="2">
+        <v>168</v>
+      </c>
+      <c r="P101" t="s" s="2">
+        <v>169</v>
+      </c>
+      <c r="Q101" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="R101" s="2"/>
+      <c r="S101" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="T101" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="U101" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="V101" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="W101" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="X101" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Y101" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Z101" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AA101" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AB101" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AC101" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AD101" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AE101" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AF101" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AG101" t="s" s="2">
+        <v>164</v>
+      </c>
+      <c r="AH101" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI101" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AJ101" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AK101" t="s" s="2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="s" s="2">
+        <v>425</v>
+      </c>
+      <c r="B102" t="s" s="2">
+        <v>170</v>
+      </c>
+      <c r="C102" t="s" s="2">
+        <v>170</v>
+      </c>
+      <c r="D102" s="2"/>
+      <c r="E102" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="F102" s="2"/>
+      <c r="G102" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="H102" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="I102" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="J102" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="K102" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="L102" t="s" s="2">
+        <v>171</v>
+      </c>
+      <c r="M102" t="s" s="2">
+        <v>172</v>
+      </c>
+      <c r="N102" t="s" s="2">
+        <v>173</v>
+      </c>
+      <c r="O102" t="s" s="2">
+        <v>174</v>
+      </c>
+      <c r="P102" t="s" s="2">
+        <v>175</v>
+      </c>
+      <c r="Q102" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="R102" s="2"/>
+      <c r="S102" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="T102" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="U102" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="V102" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="W102" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="X102" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Y102" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Z102" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AA102" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AB102" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AC102" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AD102" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AE102" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AF102" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AG102" t="s" s="2">
+        <v>170</v>
+      </c>
+      <c r="AH102" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI102" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AJ102" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AK102" t="s" s="2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="s" s="2">
+        <v>425</v>
+      </c>
+      <c r="B103" t="s" s="2">
+        <v>176</v>
+      </c>
+      <c r="C103" t="s" s="2">
+        <v>176</v>
+      </c>
+      <c r="D103" s="2"/>
+      <c r="E103" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="F103" s="2"/>
+      <c r="G103" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="H103" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I103" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="J103" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="K103" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="L103" t="s" s="2">
+        <v>177</v>
+      </c>
+      <c r="M103" t="s" s="2">
+        <v>178</v>
+      </c>
+      <c r="N103" t="s" s="2">
+        <v>179</v>
+      </c>
+      <c r="O103" t="s" s="2">
+        <v>180</v>
+      </c>
+      <c r="P103" t="s" s="2">
+        <v>181</v>
+      </c>
+      <c r="Q103" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="R103" s="2"/>
+      <c r="S103" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="T103" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="U103" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="V103" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="W103" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="X103" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Y103" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Z103" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AA103" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AB103" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AC103" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AD103" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AE103" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AF103" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AG103" t="s" s="2">
+        <v>176</v>
+      </c>
+      <c r="AH103" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI103" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ103" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AK103" t="s" s="2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="s" s="2">
+        <v>425</v>
+      </c>
+      <c r="B104" t="s" s="2">
+        <v>182</v>
+      </c>
+      <c r="C104" t="s" s="2">
+        <v>182</v>
+      </c>
+      <c r="D104" s="2"/>
+      <c r="E104" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="F104" s="2"/>
+      <c r="G104" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="H104" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="I104" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="J104" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="K104" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="L104" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="M104" t="s" s="2">
+        <v>183</v>
+      </c>
+      <c r="N104" t="s" s="2">
+        <v>184</v>
+      </c>
+      <c r="O104" s="2"/>
+      <c r="P104" t="s" s="2">
+        <v>185</v>
+      </c>
+      <c r="Q104" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="R104" s="2"/>
+      <c r="S104" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="T104" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="U104" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="V104" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="W104" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="X104" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Y104" t="s" s="2">
+        <v>66</v>
+      </c>
+      <c r="Z104" t="s" s="2">
+        <v>186</v>
+      </c>
+      <c r="AA104" t="s" s="2">
+        <v>187</v>
+      </c>
+      <c r="AB104" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AC104" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AD104" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AE104" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AF104" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AG104" t="s" s="2">
+        <v>182</v>
+      </c>
+      <c r="AH104" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI104" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AJ104" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AK104" t="s" s="2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="s" s="2">
+        <v>425</v>
+      </c>
+      <c r="B105" t="s" s="2">
+        <v>188</v>
+      </c>
+      <c r="C105" t="s" s="2">
+        <v>188</v>
+      </c>
+      <c r="D105" s="2"/>
+      <c r="E105" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="F105" s="2"/>
+      <c r="G105" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="H105" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="I105" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="J105" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="K105" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="L105" t="s" s="2">
+        <v>189</v>
+      </c>
+      <c r="M105" t="s" s="2">
+        <v>190</v>
+      </c>
+      <c r="N105" t="s" s="2">
+        <v>191</v>
+      </c>
+      <c r="O105" t="s" s="2">
+        <v>192</v>
+      </c>
+      <c r="P105" t="s" s="2">
+        <v>193</v>
+      </c>
+      <c r="Q105" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="R105" s="2"/>
+      <c r="S105" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="T105" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="U105" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="V105" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="W105" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="X105" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Y105" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Z105" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AA105" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AB105" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AC105" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AD105" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AE105" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AF105" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AG105" t="s" s="2">
+        <v>188</v>
+      </c>
+      <c r="AH105" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI105" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AJ105" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AK105" t="s" s="2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="s" s="2">
+        <v>425</v>
+      </c>
+      <c r="B106" t="s" s="2">
+        <v>194</v>
+      </c>
+      <c r="C106" t="s" s="2">
+        <v>194</v>
+      </c>
+      <c r="D106" s="2"/>
+      <c r="E106" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="F106" s="2"/>
+      <c r="G106" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="H106" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I106" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="J106" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="K106" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="L106" t="s" s="2">
+        <v>195</v>
+      </c>
+      <c r="M106" t="s" s="2">
+        <v>196</v>
+      </c>
+      <c r="N106" t="s" s="2">
+        <v>197</v>
+      </c>
+      <c r="O106" t="s" s="2">
+        <v>198</v>
+      </c>
+      <c r="P106" t="s" s="2">
+        <v>199</v>
+      </c>
+      <c r="Q106" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="R106" s="2"/>
+      <c r="S106" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="T106" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="U106" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="V106" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="W106" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="X106" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Y106" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Z106" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AA106" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AB106" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AC106" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AD106" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AE106" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AF106" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AG106" t="s" s="2">
+        <v>194</v>
+      </c>
+      <c r="AH106" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI106" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ106" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AK106" t="s" s="2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="s" s="2">
+        <v>425</v>
+      </c>
+      <c r="B107" t="s" s="2">
+        <v>200</v>
+      </c>
+      <c r="C107" t="s" s="2">
+        <v>200</v>
+      </c>
+      <c r="D107" s="2"/>
+      <c r="E107" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="F107" s="2"/>
+      <c r="G107" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="H107" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I107" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="J107" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="K107" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="L107" t="s" s="2">
+        <v>201</v>
+      </c>
+      <c r="M107" t="s" s="2">
+        <v>202</v>
+      </c>
+      <c r="N107" t="s" s="2">
+        <v>203</v>
+      </c>
+      <c r="O107" t="s" s="2">
+        <v>204</v>
+      </c>
+      <c r="P107" t="s" s="2">
+        <v>205</v>
+      </c>
+      <c r="Q107" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="R107" s="2"/>
+      <c r="S107" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="T107" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="U107" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="V107" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="W107" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="X107" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Y107" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Z107" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AA107" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AB107" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AC107" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AD107" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AE107" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AF107" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AG107" t="s" s="2">
+        <v>200</v>
+      </c>
+      <c r="AH107" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI107" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ107" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AK107" t="s" s="2">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="s" s="2">
+        <v>425</v>
+      </c>
+      <c r="B108" t="s" s="2">
+        <v>207</v>
+      </c>
+      <c r="C108" t="s" s="2">
+        <v>207</v>
+      </c>
+      <c r="D108" s="2"/>
+      <c r="E108" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="F108" s="2"/>
+      <c r="G108" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="H108" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="I108" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="J108" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="K108" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="L108" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="M108" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="N108" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="O108" s="2"/>
+      <c r="P108" s="2"/>
+      <c r="Q108" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="R108" s="2"/>
+      <c r="S108" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="T108" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="U108" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="V108" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="W108" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="X108" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Y108" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Z108" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AA108" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AB108" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AC108" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AD108" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AE108" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AF108" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AG108" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="AH108" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI108" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AJ108" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AK108" t="s" s="2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="s" s="2">
+        <v>425</v>
+      </c>
+      <c r="B109" t="s" s="2">
+        <v>208</v>
+      </c>
+      <c r="C109" t="s" s="2">
+        <v>208</v>
+      </c>
+      <c r="D109" s="2"/>
+      <c r="E109" t="s" s="2">
+        <v>126</v>
+      </c>
+      <c r="F109" s="2"/>
+      <c r="G109" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="H109" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I109" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="J109" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="K109" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="L109" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="M109" t="s" s="2">
+        <v>209</v>
+      </c>
+      <c r="N109" t="s" s="2">
+        <v>210</v>
+      </c>
+      <c r="O109" t="s" s="2">
+        <v>129</v>
+      </c>
+      <c r="P109" s="2"/>
+      <c r="Q109" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="R109" s="2"/>
+      <c r="S109" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="T109" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="U109" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="V109" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="W109" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="X109" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Y109" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Z109" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AA109" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AB109" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AC109" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AD109" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AE109" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AF109" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AG109" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="AH109" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI109" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ109" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AK109" t="s" s="2">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="s" s="2">
+        <v>425</v>
+      </c>
+      <c r="B110" t="s" s="2">
+        <v>211</v>
+      </c>
+      <c r="C110" t="s" s="2">
+        <v>211</v>
+      </c>
+      <c r="D110" s="2"/>
+      <c r="E110" t="s" s="2">
+        <v>212</v>
+      </c>
+      <c r="F110" s="2"/>
+      <c r="G110" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="H110" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I110" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="J110" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="K110" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="L110" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="M110" t="s" s="2">
+        <v>213</v>
+      </c>
+      <c r="N110" t="s" s="2">
+        <v>214</v>
+      </c>
+      <c r="O110" t="s" s="2">
+        <v>129</v>
+      </c>
+      <c r="P110" t="s" s="2">
+        <v>130</v>
+      </c>
+      <c r="Q110" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="R110" s="2"/>
+      <c r="S110" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="T110" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="U110" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="V110" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="W110" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="X110" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Y110" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Z110" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AA110" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AB110" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AC110" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AD110" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AE110" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AF110" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AG110" t="s" s="2">
+        <v>215</v>
+      </c>
+      <c r="AH110" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI110" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ110" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AK110" t="s" s="2">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="s" s="2">
+        <v>425</v>
+      </c>
+      <c r="B111" t="s" s="2">
+        <v>216</v>
+      </c>
+      <c r="C111" t="s" s="2">
+        <v>216</v>
+      </c>
+      <c r="D111" s="2"/>
+      <c r="E111" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="F111" s="2"/>
+      <c r="G111" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="H111" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I111" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="J111" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="K111" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="L111" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="M111" t="s" s="2">
+        <v>217</v>
+      </c>
+      <c r="N111" t="s" s="2">
+        <v>218</v>
+      </c>
+      <c r="O111" s="2"/>
+      <c r="P111" t="s" s="2">
+        <v>219</v>
+      </c>
+      <c r="Q111" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="R111" s="2"/>
+      <c r="S111" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="T111" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="U111" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="V111" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="W111" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="X111" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Y111" t="s" s="2">
+        <v>66</v>
+      </c>
+      <c r="Z111" t="s" s="2">
+        <v>220</v>
+      </c>
+      <c r="AA111" t="s" s="2">
+        <v>221</v>
+      </c>
+      <c r="AB111" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AC111" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AD111" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AE111" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AF111" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AG111" t="s" s="2">
+        <v>216</v>
+      </c>
+      <c r="AH111" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI111" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ111" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AK111" t="s" s="2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="s" s="2">
+        <v>425</v>
+      </c>
+      <c r="B112" t="s" s="2">
+        <v>222</v>
+      </c>
+      <c r="C112" t="s" s="2">
+        <v>222</v>
+      </c>
+      <c r="D112" s="2"/>
+      <c r="E112" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="F112" s="2"/>
+      <c r="G112" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="H112" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="I112" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="J112" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="K112" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="L112" t="s" s="2">
+        <v>145</v>
+      </c>
+      <c r="M112" t="s" s="2">
+        <v>223</v>
+      </c>
+      <c r="N112" t="s" s="2">
+        <v>224</v>
+      </c>
+      <c r="O112" s="2"/>
+      <c r="P112" t="s" s="2">
+        <v>225</v>
+      </c>
+      <c r="Q112" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="R112" s="2"/>
+      <c r="S112" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="T112" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="U112" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="V112" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="W112" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="X112" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Y112" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Z112" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AA112" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AB112" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AC112" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AD112" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AE112" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AF112" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AG112" t="s" s="2">
+        <v>222</v>
+      </c>
+      <c r="AH112" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI112" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AJ112" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AK112" t="s" s="2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="s" s="2">
+        <v>425</v>
+      </c>
+      <c r="B113" t="s" s="2">
+        <v>226</v>
+      </c>
+      <c r="C113" t="s" s="2">
+        <v>226</v>
+      </c>
+      <c r="D113" s="2"/>
+      <c r="E113" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="F113" s="2"/>
+      <c r="G113" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="H113" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I113" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="J113" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="K113" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="L113" t="s" s="2">
+        <v>151</v>
+      </c>
+      <c r="M113" t="s" s="2">
+        <v>227</v>
+      </c>
+      <c r="N113" t="s" s="2">
+        <v>228</v>
+      </c>
+      <c r="O113" t="s" s="2">
+        <v>229</v>
+      </c>
+      <c r="P113" t="s" s="2">
+        <v>155</v>
+      </c>
+      <c r="Q113" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="R113" s="2"/>
+      <c r="S113" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="T113" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="U113" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="V113" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="W113" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="X113" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Y113" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Z113" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AA113" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AB113" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AC113" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AD113" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AE113" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AF113" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AG113" t="s" s="2">
+        <v>226</v>
+      </c>
+      <c r="AH113" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI113" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ113" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AK113" t="s" s="2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="s" s="2">
+        <v>425</v>
+      </c>
+      <c r="B114" t="s" s="2">
+        <v>230</v>
+      </c>
+      <c r="C114" t="s" s="2">
+        <v>230</v>
+      </c>
+      <c r="D114" s="2"/>
+      <c r="E114" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="F114" s="2"/>
+      <c r="G114" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="H114" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="I114" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="J114" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="K114" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="L114" t="s" s="2">
+        <v>177</v>
+      </c>
+      <c r="M114" t="s" s="2">
+        <v>231</v>
+      </c>
+      <c r="N114" t="s" s="2">
+        <v>232</v>
+      </c>
+      <c r="O114" s="2"/>
+      <c r="P114" t="s" s="2">
+        <v>233</v>
+      </c>
+      <c r="Q114" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="R114" s="2"/>
+      <c r="S114" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="T114" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="U114" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="V114" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="W114" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="X114" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Y114" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Z114" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AA114" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AB114" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AC114" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AD114" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AE114" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AF114" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AG114" t="s" s="2">
+        <v>230</v>
+      </c>
+      <c r="AH114" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI114" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AJ114" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AK114" t="s" s="2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="s" s="2">
+        <v>425</v>
+      </c>
+      <c r="B115" t="s" s="2">
+        <v>234</v>
+      </c>
+      <c r="C115" t="s" s="2">
+        <v>234</v>
+      </c>
+      <c r="D115" s="2"/>
+      <c r="E115" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="F115" s="2"/>
+      <c r="G115" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="H115" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="I115" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="J115" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="K115" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="L115" t="s" s="2">
+        <v>98</v>
+      </c>
+      <c r="M115" t="s" s="2">
+        <v>157</v>
+      </c>
+      <c r="N115" t="s" s="2">
+        <v>235</v>
+      </c>
+      <c r="O115" s="2"/>
+      <c r="P115" t="s" s="2">
+        <v>236</v>
+      </c>
+      <c r="Q115" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="R115" s="2"/>
+      <c r="S115" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="T115" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="U115" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="V115" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="W115" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="X115" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Y115" t="s" s="2">
+        <v>161</v>
+      </c>
+      <c r="Z115" t="s" s="2">
+        <v>162</v>
+      </c>
+      <c r="AA115" t="s" s="2">
+        <v>163</v>
+      </c>
+      <c r="AB115" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AC115" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AD115" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AE115" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AF115" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AG115" t="s" s="2">
+        <v>234</v>
+      </c>
+      <c r="AH115" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI115" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AJ115" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AK115" t="s" s="2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="s" s="2">
+        <v>425</v>
+      </c>
+      <c r="B116" t="s" s="2">
+        <v>237</v>
+      </c>
+      <c r="C116" t="s" s="2">
+        <v>237</v>
+      </c>
+      <c r="D116" s="2"/>
+      <c r="E116" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="F116" s="2"/>
+      <c r="G116" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="H116" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="I116" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="J116" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="K116" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="L116" t="s" s="2">
+        <v>238</v>
+      </c>
+      <c r="M116" t="s" s="2">
+        <v>239</v>
+      </c>
+      <c r="N116" t="s" s="2">
+        <v>240</v>
+      </c>
+      <c r="O116" s="2"/>
+      <c r="P116" t="s" s="2">
+        <v>241</v>
+      </c>
+      <c r="Q116" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="R116" s="2"/>
+      <c r="S116" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="T116" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="U116" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="V116" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="W116" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="X116" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Y116" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Z116" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AA116" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AB116" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AC116" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AD116" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AE116" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AF116" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AG116" t="s" s="2">
+        <v>237</v>
+      </c>
+      <c r="AH116" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI116" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AJ116" t="s" s="2">
+        <v>242</v>
+      </c>
+      <c r="AK116" t="s" s="2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="s" s="2">
+        <v>425</v>
+      </c>
+      <c r="B117" t="s" s="2">
+        <v>243</v>
+      </c>
+      <c r="C117" t="s" s="2">
+        <v>243</v>
+      </c>
+      <c r="D117" s="2"/>
+      <c r="E117" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="F117" s="2"/>
+      <c r="G117" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="H117" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="I117" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="J117" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="K117" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="L117" t="s" s="2">
+        <v>244</v>
+      </c>
+      <c r="M117" t="s" s="2">
+        <v>245</v>
+      </c>
+      <c r="N117" t="s" s="2">
+        <v>246</v>
+      </c>
+      <c r="O117" s="2"/>
+      <c r="P117" s="2"/>
+      <c r="Q117" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="R117" s="2"/>
+      <c r="S117" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="T117" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="U117" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="V117" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="W117" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="X117" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Y117" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Z117" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AA117" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AB117" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AC117" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AD117" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AE117" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AF117" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AG117" t="s" s="2">
+        <v>243</v>
+      </c>
+      <c r="AH117" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI117" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AJ117" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AK117" t="s" s="2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="s" s="2">
+        <v>425</v>
+      </c>
+      <c r="B118" t="s" s="2">
+        <v>247</v>
+      </c>
+      <c r="C118" t="s" s="2">
+        <v>247</v>
+      </c>
+      <c r="D118" s="2"/>
+      <c r="E118" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="F118" s="2"/>
+      <c r="G118" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="H118" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I118" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="J118" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="K118" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="L118" t="s" s="2">
+        <v>201</v>
+      </c>
+      <c r="M118" t="s" s="2">
+        <v>248</v>
+      </c>
+      <c r="N118" t="s" s="2">
+        <v>249</v>
+      </c>
+      <c r="O118" t="s" s="2">
+        <v>250</v>
+      </c>
+      <c r="P118" t="s" s="2">
+        <v>251</v>
+      </c>
+      <c r="Q118" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="R118" s="2"/>
+      <c r="S118" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="T118" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="U118" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="V118" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="W118" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="X118" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Y118" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Z118" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AA118" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AB118" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AC118" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AD118" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AE118" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AF118" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AG118" t="s" s="2">
+        <v>247</v>
+      </c>
+      <c r="AH118" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI118" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ118" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AK118" t="s" s="2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="s" s="2">
+        <v>425</v>
+      </c>
+      <c r="B119" t="s" s="2">
+        <v>252</v>
+      </c>
+      <c r="C119" t="s" s="2">
+        <v>252</v>
+      </c>
+      <c r="D119" s="2"/>
+      <c r="E119" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="F119" s="2"/>
+      <c r="G119" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="H119" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="I119" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="J119" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="K119" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="L119" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="M119" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="N119" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="O119" s="2"/>
+      <c r="P119" s="2"/>
+      <c r="Q119" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="R119" s="2"/>
+      <c r="S119" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="T119" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="U119" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="V119" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="W119" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="X119" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Y119" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Z119" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AA119" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AB119" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AC119" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AD119" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AE119" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AF119" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AG119" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="AH119" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI119" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AJ119" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AK119" t="s" s="2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="s" s="2">
+        <v>425</v>
+      </c>
+      <c r="B120" t="s" s="2">
+        <v>253</v>
+      </c>
+      <c r="C120" t="s" s="2">
+        <v>253</v>
+      </c>
+      <c r="D120" s="2"/>
+      <c r="E120" t="s" s="2">
+        <v>126</v>
+      </c>
+      <c r="F120" s="2"/>
+      <c r="G120" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="H120" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I120" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="J120" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="K120" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="L120" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="M120" t="s" s="2">
+        <v>209</v>
+      </c>
+      <c r="N120" t="s" s="2">
+        <v>210</v>
+      </c>
+      <c r="O120" t="s" s="2">
+        <v>129</v>
+      </c>
+      <c r="P120" s="2"/>
+      <c r="Q120" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="R120" s="2"/>
+      <c r="S120" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="T120" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="U120" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="V120" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="W120" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="X120" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Y120" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Z120" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AA120" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AB120" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AC120" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AD120" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AE120" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AF120" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AG120" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="AH120" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI120" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ120" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AK120" t="s" s="2">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="s" s="2">
+        <v>425</v>
+      </c>
+      <c r="B121" t="s" s="2">
+        <v>254</v>
+      </c>
+      <c r="C121" t="s" s="2">
+        <v>254</v>
+      </c>
+      <c r="D121" s="2"/>
+      <c r="E121" t="s" s="2">
+        <v>212</v>
+      </c>
+      <c r="F121" s="2"/>
+      <c r="G121" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="H121" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I121" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="J121" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="K121" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="L121" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="M121" t="s" s="2">
+        <v>213</v>
+      </c>
+      <c r="N121" t="s" s="2">
+        <v>214</v>
+      </c>
+      <c r="O121" t="s" s="2">
+        <v>129</v>
+      </c>
+      <c r="P121" t="s" s="2">
+        <v>130</v>
+      </c>
+      <c r="Q121" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="R121" s="2"/>
+      <c r="S121" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="T121" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="U121" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="V121" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="W121" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="X121" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Y121" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Z121" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AA121" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AB121" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AC121" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AD121" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AE121" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AF121" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AG121" t="s" s="2">
+        <v>215</v>
+      </c>
+      <c r="AH121" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI121" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ121" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AK121" t="s" s="2">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="s" s="2">
+        <v>425</v>
+      </c>
+      <c r="B122" t="s" s="2">
+        <v>255</v>
+      </c>
+      <c r="C122" t="s" s="2">
+        <v>255</v>
+      </c>
+      <c r="D122" s="2"/>
+      <c r="E122" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="F122" s="2"/>
+      <c r="G122" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="H122" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="I122" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="J122" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="K122" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="L122" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="M122" t="s" s="2">
+        <v>256</v>
+      </c>
+      <c r="N122" t="s" s="2">
+        <v>257</v>
+      </c>
+      <c r="O122" t="s" s="2">
+        <v>258</v>
+      </c>
+      <c r="P122" t="s" s="2">
+        <v>259</v>
+      </c>
+      <c r="Q122" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="R122" s="2"/>
+      <c r="S122" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="T122" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="U122" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="V122" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="W122" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="X122" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Y122" t="s" s="2">
+        <v>102</v>
+      </c>
+      <c r="Z122" t="s" s="2">
+        <v>103</v>
+      </c>
+      <c r="AA122" t="s" s="2">
+        <v>104</v>
+      </c>
+      <c r="AB122" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AC122" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AD122" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AE122" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AF122" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AG122" t="s" s="2">
+        <v>255</v>
+      </c>
+      <c r="AH122" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AI122" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AJ122" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AK122" t="s" s="2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="s" s="2">
+        <v>425</v>
+      </c>
+      <c r="B123" t="s" s="2">
+        <v>260</v>
+      </c>
+      <c r="C123" t="s" s="2">
+        <v>260</v>
+      </c>
+      <c r="D123" s="2"/>
+      <c r="E123" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="F123" s="2"/>
+      <c r="G123" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="H123" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="I123" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="J123" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="K123" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="L123" t="s" s="2">
+        <v>138</v>
+      </c>
+      <c r="M123" t="s" s="2">
+        <v>261</v>
+      </c>
+      <c r="N123" t="s" s="2">
+        <v>262</v>
+      </c>
+      <c r="O123" t="s" s="2">
+        <v>263</v>
+      </c>
+      <c r="P123" t="s" s="2">
+        <v>264</v>
+      </c>
+      <c r="Q123" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="R123" s="2"/>
+      <c r="S123" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="T123" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="U123" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="V123" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="W123" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="X123" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Y123" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Z123" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AA123" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AB123" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AC123" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AD123" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AE123" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AF123" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AG123" t="s" s="2">
+        <v>260</v>
+      </c>
+      <c r="AH123" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI123" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AJ123" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AK123" t="s" s="2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="s" s="2">
+        <v>425</v>
+      </c>
+      <c r="B124" t="s" s="2">
+        <v>265</v>
+      </c>
+      <c r="C124" t="s" s="2">
+        <v>265</v>
+      </c>
+      <c r="D124" s="2"/>
+      <c r="E124" t="s" s="2">
+        <v>266</v>
+      </c>
+      <c r="F124" s="2"/>
+      <c r="G124" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="H124" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I124" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="J124" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="K124" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="L124" t="s" s="2">
+        <v>267</v>
+      </c>
+      <c r="M124" t="s" s="2">
+        <v>268</v>
+      </c>
+      <c r="N124" t="s" s="2">
+        <v>269</v>
+      </c>
+      <c r="O124" t="s" s="2">
+        <v>270</v>
+      </c>
+      <c r="P124" s="2"/>
+      <c r="Q124" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="R124" s="2"/>
+      <c r="S124" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="T124" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="U124" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="V124" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="W124" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="X124" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Y124" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Z124" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AA124" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AB124" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AC124" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AD124" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AE124" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AF124" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AG124" t="s" s="2">
+        <v>265</v>
+      </c>
+      <c r="AH124" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI124" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ124" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AK124" t="s" s="2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="s" s="2">
+        <v>425</v>
+      </c>
+      <c r="B125" t="s" s="2">
+        <v>271</v>
+      </c>
+      <c r="C125" t="s" s="2">
+        <v>271</v>
+      </c>
+      <c r="D125" s="2"/>
+      <c r="E125" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="F125" s="2"/>
+      <c r="G125" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="H125" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="I125" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="J125" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="K125" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="L125" t="s" s="2">
+        <v>238</v>
+      </c>
+      <c r="M125" t="s" s="2">
+        <v>272</v>
+      </c>
+      <c r="N125" t="s" s="2">
+        <v>273</v>
+      </c>
+      <c r="O125" t="s" s="2">
+        <v>274</v>
+      </c>
+      <c r="P125" t="s" s="2">
+        <v>275</v>
+      </c>
+      <c r="Q125" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="R125" s="2"/>
+      <c r="S125" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="T125" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="U125" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="V125" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="W125" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="X125" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Y125" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Z125" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AA125" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AB125" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AC125" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AD125" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AE125" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AF125" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AG125" t="s" s="2">
+        <v>271</v>
+      </c>
+      <c r="AH125" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI125" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AJ125" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AK125" t="s" s="2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="s" s="2">
+        <v>425</v>
+      </c>
+      <c r="B126" t="s" s="2">
+        <v>276</v>
+      </c>
+      <c r="C126" t="s" s="2">
+        <v>276</v>
+      </c>
+      <c r="D126" s="2"/>
+      <c r="E126" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="F126" s="2"/>
+      <c r="G126" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="H126" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I126" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="J126" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="K126" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="L126" t="s" s="2">
+        <v>201</v>
+      </c>
+      <c r="M126" t="s" s="2">
+        <v>277</v>
+      </c>
+      <c r="N126" t="s" s="2">
+        <v>278</v>
+      </c>
+      <c r="O126" t="s" s="2">
+        <v>279</v>
+      </c>
+      <c r="P126" t="s" s="2">
+        <v>280</v>
+      </c>
+      <c r="Q126" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="R126" s="2"/>
+      <c r="S126" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="T126" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="U126" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="V126" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="W126" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="X126" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Y126" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Z126" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AA126" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AB126" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AC126" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AD126" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AE126" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AF126" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AG126" t="s" s="2">
+        <v>276</v>
+      </c>
+      <c r="AH126" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI126" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ126" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AK126" t="s" s="2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="s" s="2">
+        <v>425</v>
+      </c>
+      <c r="B127" t="s" s="2">
+        <v>281</v>
+      </c>
+      <c r="C127" t="s" s="2">
+        <v>281</v>
+      </c>
+      <c r="D127" s="2"/>
+      <c r="E127" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="F127" s="2"/>
+      <c r="G127" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="H127" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="I127" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="J127" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="K127" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="L127" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="M127" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="N127" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="O127" s="2"/>
+      <c r="P127" s="2"/>
+      <c r="Q127" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="R127" s="2"/>
+      <c r="S127" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="T127" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="U127" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="V127" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="W127" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="X127" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Y127" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Z127" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AA127" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AB127" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AC127" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AD127" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AE127" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AF127" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AG127" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="AH127" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI127" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AJ127" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AK127" t="s" s="2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="s" s="2">
+        <v>425</v>
+      </c>
+      <c r="B128" t="s" s="2">
+        <v>282</v>
+      </c>
+      <c r="C128" t="s" s="2">
+        <v>282</v>
+      </c>
+      <c r="D128" s="2"/>
+      <c r="E128" t="s" s="2">
+        <v>126</v>
+      </c>
+      <c r="F128" s="2"/>
+      <c r="G128" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="H128" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I128" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="J128" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="K128" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="L128" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="M128" t="s" s="2">
+        <v>209</v>
+      </c>
+      <c r="N128" t="s" s="2">
+        <v>210</v>
+      </c>
+      <c r="O128" t="s" s="2">
+        <v>129</v>
+      </c>
+      <c r="P128" s="2"/>
+      <c r="Q128" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="R128" s="2"/>
+      <c r="S128" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="T128" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="U128" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="V128" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="W128" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="X128" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Y128" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Z128" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AA128" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AB128" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AC128" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AD128" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AE128" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AF128" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AG128" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="AH128" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI128" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ128" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AK128" t="s" s="2">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="s" s="2">
+        <v>425</v>
+      </c>
+      <c r="B129" t="s" s="2">
+        <v>283</v>
+      </c>
+      <c r="C129" t="s" s="2">
+        <v>283</v>
+      </c>
+      <c r="D129" s="2"/>
+      <c r="E129" t="s" s="2">
+        <v>212</v>
+      </c>
+      <c r="F129" s="2"/>
+      <c r="G129" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="H129" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I129" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="J129" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="K129" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="L129" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="M129" t="s" s="2">
+        <v>213</v>
+      </c>
+      <c r="N129" t="s" s="2">
+        <v>214</v>
+      </c>
+      <c r="O129" t="s" s="2">
+        <v>129</v>
+      </c>
+      <c r="P129" t="s" s="2">
+        <v>130</v>
+      </c>
+      <c r="Q129" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="R129" s="2"/>
+      <c r="S129" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="T129" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="U129" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="V129" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="W129" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="X129" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Y129" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Z129" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AA129" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AB129" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AC129" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AD129" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AE129" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AF129" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AG129" t="s" s="2">
+        <v>215</v>
+      </c>
+      <c r="AH129" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI129" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ129" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AK129" t="s" s="2">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="s" s="2">
+        <v>425</v>
+      </c>
+      <c r="B130" t="s" s="2">
+        <v>284</v>
+      </c>
+      <c r="C130" t="s" s="2">
+        <v>284</v>
+      </c>
+      <c r="D130" s="2"/>
+      <c r="E130" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="F130" s="2"/>
+      <c r="G130" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="H130" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="I130" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="J130" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="K130" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="L130" t="s" s="2">
+        <v>285</v>
+      </c>
+      <c r="M130" t="s" s="2">
+        <v>286</v>
+      </c>
+      <c r="N130" t="s" s="2">
+        <v>287</v>
+      </c>
+      <c r="O130" t="s" s="2">
+        <v>288</v>
+      </c>
+      <c r="P130" s="2"/>
+      <c r="Q130" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="R130" s="2"/>
+      <c r="S130" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="T130" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="U130" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="V130" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="W130" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="X130" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Y130" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Z130" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AA130" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AB130" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AC130" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AD130" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AE130" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AF130" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AG130" t="s" s="2">
+        <v>284</v>
+      </c>
+      <c r="AH130" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AI130" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AJ130" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AK130" t="s" s="2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="s" s="2">
+        <v>425</v>
+      </c>
+      <c r="B131" t="s" s="2">
+        <v>289</v>
+      </c>
+      <c r="C131" t="s" s="2">
+        <v>289</v>
+      </c>
+      <c r="D131" s="2"/>
+      <c r="E131" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="F131" s="2"/>
+      <c r="G131" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="H131" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="I131" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="J131" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="K131" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="L131" t="s" s="2">
+        <v>98</v>
+      </c>
+      <c r="M131" t="s" s="2">
+        <v>290</v>
+      </c>
+      <c r="N131" t="s" s="2">
+        <v>291</v>
+      </c>
+      <c r="O131" s="2"/>
+      <c r="P131" s="2"/>
+      <c r="Q131" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="R131" s="2"/>
+      <c r="S131" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="T131" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="U131" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="V131" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="W131" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="X131" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="Y131" t="s" s="2">
+        <v>161</v>
+      </c>
+      <c r="Z131" t="s" s="2">
+        <v>291</v>
+      </c>
+      <c r="AA131" t="s" s="2">
+        <v>292</v>
+      </c>
+      <c r="AB131" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AC131" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AD131" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AE131" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AF131" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AG131" t="s" s="2">
+        <v>289</v>
+      </c>
+      <c r="AH131" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AI131" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AJ131" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AK131" t="s" s="2">
+        <v>68</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>